<commit_message>
Calculations to determine an area for each targeted tree
</commit_message>
<xml_diff>
--- a/15N_experiment/Canopy_surface_models_calculations.xlsx
+++ b/15N_experiment/Canopy_surface_models_calculations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="13">
   <si>
     <t>distance from trees</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>STAR reviewed = area by mean distance + (area by gamma - area by mean distance)/2</t>
+  </si>
+  <si>
+    <t>Corrected by 1/6 (i.e. 1/3 of half of the canopy being damaged by wires and hence "lighter")</t>
   </si>
 </sst>
 </file>
@@ -67,7 +70,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -114,13 +117,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,7 +408,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,7 +417,7 @@
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -430,7 +434,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -441,7 +445,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -452,7 +456,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -463,7 +467,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -477,7 +481,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -491,7 +495,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -505,7 +509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -513,12 +517,12 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -531,7 +535,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -543,8 +547,11 @@
         <f>D10^2*PI()</f>
         <v>24.630086404143974</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -556,8 +563,12 @@
         <f>C11+(E11-C11)/2</f>
         <v>17.357408494161856</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12" s="6">
+        <f>D12*5/6</f>
+        <v>13.79905484986277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -568,7 +579,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -582,7 +593,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -682,7 +693,7 @@
         <f>AVERAGE(B22,D22)^2*PI()</f>
         <v>11.847653656639201</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="6">
         <f>C23+(E23-C23)/2</f>
         <v>12.870276626909</v>
       </c>
@@ -819,7 +830,7 @@
         <f>AVERAGE(B34,D34)^2*PI()</f>
         <v>11.532628157856115</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="6">
         <f>C35+(E35-C35)/2</f>
         <v>12.109388268630829</v>
       </c>

</xml_diff>